<commit_message>
Finalización de puntos 4 y 5
Finalización y ajustes del documento. Creación del README.
</commit_message>
<xml_diff>
--- a/Tablas_graficos/Tablas.xlsx
+++ b/Tablas_graficos/Tablas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Desktop/Problem_set_1_WS_JSV/Tablas_graficos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a9af9f48e27c989/Documentos/Maestría en Economía Aplicada/Big Data/GitHub/Talleres/Problem_set_1_WS_JSV/Tablas_graficos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A0F010-29C7-B249-A407-4D9BD67B54D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{07A0F010-29C7-B249-A407-4D9BD67B54D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32F5E249-B235-455E-95AC-E55DA7748C02}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{A9AD60D7-42D7-8D4E-9221-6A8F0041E1FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9AD60D7-42D7-8D4E-9221-6A8F0041E1FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>mean</t>
   </si>
@@ -150,59 +151,68 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>Bootstrap Statistics :</t>
-  </si>
-  <si>
-    <t>original</t>
-  </si>
-  <si>
-    <t>bias</t>
-  </si>
-  <si>
-    <t>std. error</t>
-  </si>
-  <si>
-    <t>t1*</t>
-  </si>
-  <si>
-    <t>t2*</t>
-  </si>
-  <si>
-    <t>t3*</t>
-  </si>
-  <si>
-    <t>t4*</t>
-  </si>
-  <si>
-    <t>t5*</t>
-  </si>
-  <si>
-    <t>t6*</t>
-  </si>
-  <si>
-    <t>Bootstrap Statistics mujeres:</t>
-  </si>
-  <si>
-    <t>Bootstrap Statistics hombres:</t>
-  </si>
-  <si>
-    <t>Lim_superior</t>
-  </si>
-  <si>
-    <t>Lim_inferior</t>
-  </si>
-  <si>
-    <t>riginal</t>
+    <t>Lim. Inferior</t>
+  </si>
+  <si>
+    <t>Lim. Superior</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>Coeficientes</t>
+  </si>
+  <si>
+    <t>Estadísticos del Bootstrap</t>
+  </si>
+  <si>
+    <t>Estadísticos del Bootstrap. Modelo mujeres</t>
+  </si>
+  <si>
+    <t>Estadísticos del Bootstrap: modelo hombres</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>Error estándar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -216,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -246,7 +256,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -258,13 +268,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -273,13 +298,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -291,9 +331,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -303,12 +341,23 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -321,7 +370,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -336,7 +385,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -351,7 +400,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -363,95 +412,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -460,7 +427,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -471,52 +440,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -526,50 +449,44 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,64 +511,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,20 +863,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3000ED6-8A9F-9240-B305-4BA925E95566}">
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A34:E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.83203125" customWidth="1"/>
+    <col min="26" max="26" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>37</v>
       </c>
@@ -1011,55 +907,35 @@
       <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="26" t="s">
+      <c r="O1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="T1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AD1" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="38"/>
-      <c r="AI1" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="38"/>
-    </row>
-    <row r="2" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1090,72 +966,35 @@
       <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="21">
-        <v>0</v>
-      </c>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="20">
+        <v>0</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="21">
+      <c r="P2" s="20">
         <v>18</v>
       </c>
-      <c r="Q2" s="21">
+      <c r="Q2" s="20">
         <v>28</v>
       </c>
-      <c r="R2" s="21">
+      <c r="R2" s="20">
         <v>38</v>
       </c>
-      <c r="S2" s="21">
+      <c r="S2" s="20">
         <v>50</v>
       </c>
-      <c r="T2" s="22">
+      <c r="T2" s="21">
         <v>93</v>
       </c>
-      <c r="W2" s="33"/>
-      <c r="X2" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA2" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF2" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG2" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK2" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL2" s="41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1025,7 @@
       <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="M3" s="13">
@@ -1210,47 +1049,11 @@
       <c r="S3" s="13">
         <v>1750703</v>
       </c>
-      <c r="T3" s="16">
+      <c r="T3" s="15">
         <v>85833333</v>
       </c>
-      <c r="W3" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="X3" s="31">
-        <v>-4809133000000</v>
-      </c>
-      <c r="Y3" s="31">
-        <v>-21144190000</v>
-      </c>
-      <c r="Z3" s="32">
-        <v>22767472857</v>
-      </c>
-      <c r="AD3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE3" s="42">
-        <v>10804400</v>
-      </c>
-      <c r="AF3" s="42">
-        <v>4443.0929999999998</v>
-      </c>
-      <c r="AG3" s="43">
-        <v>109092.4</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ3" s="42">
-        <v>10988560</v>
-      </c>
-      <c r="AK3" s="42">
-        <v>-577.81219999999996</v>
-      </c>
-      <c r="AL3" s="43">
-        <v>91198.38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1281,7 +1084,7 @@
       <c r="J4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="13">
@@ -1305,47 +1108,11 @@
       <c r="S4" s="13">
         <v>6</v>
       </c>
-      <c r="T4" s="16">
+      <c r="T4" s="15">
         <v>9</v>
       </c>
-      <c r="W4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="27">
-        <v>81327340000</v>
-      </c>
-      <c r="Y4" s="27">
-        <v>1209575000</v>
-      </c>
-      <c r="Z4" s="28">
-        <v>1172157550</v>
-      </c>
-      <c r="AD4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE4" s="27">
-        <v>47058.03</v>
-      </c>
-      <c r="AF4" s="27">
-        <v>-343.87970000000001</v>
-      </c>
-      <c r="AG4" s="44">
-        <v>4772.2879999999996</v>
-      </c>
-      <c r="AI4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ4" s="27">
-        <v>61268.98</v>
-      </c>
-      <c r="AK4" s="27">
-        <v>120.28440000000001</v>
-      </c>
-      <c r="AL4" s="44">
-        <v>4125.1450000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1376,7 +1143,7 @@
       <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="13">
@@ -1400,47 +1167,11 @@
       <c r="S5" s="13">
         <v>1</v>
       </c>
-      <c r="T5" s="16">
+      <c r="T5" s="15">
         <v>6</v>
       </c>
-      <c r="W5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="X5" s="27">
-        <v>-545214800</v>
-      </c>
-      <c r="Y5" s="27">
-        <v>-13892890</v>
-      </c>
-      <c r="Z5" s="28">
-        <v>14769733</v>
-      </c>
-      <c r="AD5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE5" s="27">
-        <v>-517.15949999999998</v>
-      </c>
-      <c r="AF5" s="27">
-        <v>3.965373</v>
-      </c>
-      <c r="AG5" s="44">
-        <v>58.3371</v>
-      </c>
-      <c r="AI5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ5" s="27">
-        <v>-588.89480000000003</v>
-      </c>
-      <c r="AK5" s="27">
-        <v>-1.7120919999999999</v>
-      </c>
-      <c r="AL5" s="44">
-        <v>49.916440000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1471,7 +1202,7 @@
       <c r="J6" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="14" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="13">
@@ -1495,47 +1226,11 @@
       <c r="S6" s="13">
         <v>3</v>
       </c>
-      <c r="T6" s="16">
+      <c r="T6" s="15">
         <v>4</v>
       </c>
-      <c r="W6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="27">
-        <v>822174900000</v>
-      </c>
-      <c r="Y6" s="27">
-        <v>-141045700</v>
-      </c>
-      <c r="Z6" s="28">
-        <v>2320110642</v>
-      </c>
-      <c r="AD6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE6" s="27">
-        <v>386964.8</v>
-      </c>
-      <c r="AF6" s="27">
-        <v>296.25729999999999</v>
-      </c>
-      <c r="AG6" s="44">
-        <v>10721.28</v>
-      </c>
-      <c r="AI6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ6" s="27">
-        <v>320786.09999999998</v>
-      </c>
-      <c r="AK6" s="27">
-        <v>-303.43110000000001</v>
-      </c>
-      <c r="AL6" s="44">
-        <v>8403.3649999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1566,7 +1261,7 @@
       <c r="J7" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="M7" s="13">
@@ -1590,48 +1285,12 @@
       <c r="S7" s="13">
         <v>1</v>
       </c>
-      <c r="T7" s="16">
-        <v>1</v>
-      </c>
-      <c r="W7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="X7" s="27">
-        <v>3952434000</v>
-      </c>
-      <c r="Y7" s="27">
-        <v>-27501090</v>
-      </c>
-      <c r="Z7" s="28">
-        <v>94519970</v>
-      </c>
-      <c r="AD7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE7" s="27">
-        <v>2966.692</v>
-      </c>
-      <c r="AF7" s="27">
-        <v>21.888249999999999</v>
-      </c>
-      <c r="AG7" s="44">
-        <v>370.46820000000002</v>
-      </c>
-      <c r="AI7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ7" s="27">
-        <v>1982.482</v>
-      </c>
-      <c r="AK7" s="27">
-        <v>12.38114</v>
-      </c>
-      <c r="AL7" s="44">
-        <v>274.49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L8" s="15" t="s">
+      <c r="T7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="M8" s="13">
@@ -1655,81 +1314,430 @@
       <c r="S8" s="13">
         <v>84</v>
       </c>
-      <c r="T8" s="16">
+      <c r="T8" s="15">
         <v>720</v>
       </c>
-      <c r="W8" s="17" t="s">
+    </row>
+    <row r="9" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="17">
+        <v>0</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>33</v>
+      </c>
+      <c r="R9" s="17">
+        <v>45</v>
+      </c>
+      <c r="S9" s="17">
+        <v>70</v>
+      </c>
+      <c r="T9" s="18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="31">
+        <v>-4809133</v>
+      </c>
+      <c r="C16" s="32">
+        <v>227674.72857000001</v>
+      </c>
+      <c r="D16" s="32">
+        <v>-5255375.4679971999</v>
+      </c>
+      <c r="E16" s="32">
+        <v>-4362890.5320028001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="31">
+        <v>81327.34</v>
+      </c>
+      <c r="C17" s="32">
+        <v>11721.575500000001</v>
+      </c>
+      <c r="D17" s="32">
+        <v>58353.052019999996</v>
+      </c>
+      <c r="E17" s="32">
+        <v>104301.62797999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="31">
+        <v>-545.21479999999997</v>
+      </c>
+      <c r="C18" s="32">
+        <v>147.69732999999999</v>
+      </c>
+      <c r="D18" s="32">
+        <v>-834.70156679999991</v>
+      </c>
+      <c r="E18" s="32">
+        <v>-255.72803319999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="31">
+        <v>822174.9</v>
+      </c>
+      <c r="C19" s="32">
+        <v>23201.10642</v>
+      </c>
+      <c r="D19" s="32">
+        <v>776700.73141680006</v>
+      </c>
+      <c r="E19" s="32">
+        <v>867649.06858319999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="31">
+        <v>3952.4340000000002</v>
+      </c>
+      <c r="C20" s="32">
+        <v>945.19970000000001</v>
+      </c>
+      <c r="D20" s="32">
+        <v>2099.8425880000004</v>
+      </c>
+      <c r="E20" s="32">
+        <v>5805.025412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="31">
+        <v>-1.782197</v>
+      </c>
+      <c r="C21" s="32">
+        <v>3.1973099999999999</v>
+      </c>
+      <c r="D21" s="32">
+        <v>-8.0489245999999994</v>
+      </c>
+      <c r="E21" s="32">
+        <v>4.4845305999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="X8" s="29">
-        <v>-1782197</v>
-      </c>
-      <c r="Y8" s="29">
-        <v>10804.71</v>
-      </c>
-      <c r="Z8" s="30">
-        <v>319731</v>
-      </c>
-      <c r="AD8" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE8" s="29">
-        <v>-3.5377070000000002</v>
-      </c>
-      <c r="AF8" s="29">
-        <v>-7.3161229999999994E-2</v>
-      </c>
-      <c r="AG8" s="45">
-        <v>1.156285</v>
-      </c>
-      <c r="AI8" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="AJ8" s="29">
-        <v>-2.6450279999999999</v>
-      </c>
-      <c r="AK8" s="29">
-        <v>-3.757833E-2</v>
-      </c>
-      <c r="AL8" s="45">
-        <v>0.77664800000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="18">
-        <v>0</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>33</v>
-      </c>
-      <c r="R9" s="18">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+    </row>
+    <row r="25" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="S9" s="18">
-        <v>70</v>
-      </c>
-      <c r="T9" s="19">
-        <v>99</v>
+      <c r="B25" s="28"/>
+      <c r="C25" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="32">
+        <v>10.804399999999999</v>
+      </c>
+      <c r="C26" s="32">
+        <v>0.10909240000000001</v>
+      </c>
+      <c r="D26" s="32">
+        <v>10.590578895999998</v>
+      </c>
+      <c r="E26" s="32">
+        <v>11.018221104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="32">
+        <v>4.7058030000000001E-2</v>
+      </c>
+      <c r="C27" s="32">
+        <v>4.7722880000000004E-3</v>
+      </c>
+      <c r="D27" s="32">
+        <v>3.7704345520000002E-2</v>
+      </c>
+      <c r="E27" s="32">
+        <v>5.641171448E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="32">
+        <v>-5.1715949999999995E-4</v>
+      </c>
+      <c r="C28" s="32">
+        <v>5.8337100000000001E-5</v>
+      </c>
+      <c r="D28" s="32">
+        <v>-6.315002159999999E-4</v>
+      </c>
+      <c r="E28" s="32">
+        <v>-4.0281878399999995E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="32">
+        <v>0.3869648</v>
+      </c>
+      <c r="C29" s="32">
+        <v>1.072128E-2</v>
+      </c>
+      <c r="D29" s="32">
+        <v>0.36595109120000002</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0.40797850879999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="32">
+        <v>2.9666919999999999E-3</v>
+      </c>
+      <c r="C30" s="32">
+        <v>3.704682E-4</v>
+      </c>
+      <c r="D30" s="32">
+        <v>2.2405743279999999E-3</v>
+      </c>
+      <c r="E30" s="32">
+        <v>3.6928096719999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="32">
+        <v>-3.537707E-6</v>
+      </c>
+      <c r="C31" s="32">
+        <v>1.1562850000000001E-6</v>
+      </c>
+      <c r="D31" s="32">
+        <v>-5.8040256000000004E-6</v>
+      </c>
+      <c r="E31" s="32">
+        <v>-1.2713884000000001E-6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="28"/>
+    </row>
+    <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="32">
+        <v>10.98856</v>
+      </c>
+      <c r="C36" s="32">
+        <v>9.1198379999999996E-2</v>
+      </c>
+      <c r="D36" s="32">
+        <v>10.8098111752</v>
+      </c>
+      <c r="E36" s="32">
+        <v>11.167308824799999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="32">
+        <v>6.1268980000000001E-2</v>
+      </c>
+      <c r="C37" s="32">
+        <v>4.1251450000000002E-3</v>
+      </c>
+      <c r="D37" s="32">
+        <v>5.31836958E-2</v>
+      </c>
+      <c r="E37" s="32">
+        <v>6.9354264200000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="32">
+        <v>-5.8889480000000002E-4</v>
+      </c>
+      <c r="C38" s="32">
+        <v>4.9916439999999998E-5</v>
+      </c>
+      <c r="D38" s="32">
+        <v>-6.8673102240000004E-4</v>
+      </c>
+      <c r="E38" s="32">
+        <v>-4.910585776E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="32">
+        <v>0.32078610000000002</v>
+      </c>
+      <c r="C39" s="32">
+        <v>8.4033649999999994E-3</v>
+      </c>
+      <c r="D39" s="32">
+        <v>0.30431550460000001</v>
+      </c>
+      <c r="E39" s="32">
+        <v>0.33725669540000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="32">
+        <v>1.9824819999999998E-3</v>
+      </c>
+      <c r="C40" s="32">
+        <v>2.7449000000000001E-4</v>
+      </c>
+      <c r="D40" s="32">
+        <v>1.4444815999999998E-3</v>
+      </c>
+      <c r="E40" s="32">
+        <v>2.5204823999999998E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="32">
+        <v>-2.645028E-6</v>
+      </c>
+      <c r="C41" s="32">
+        <v>7.7664799999999995E-7</v>
+      </c>
+      <c r="D41" s="32">
+        <v>-4.1672580800000003E-6</v>
+      </c>
+      <c r="E41" s="32">
+        <v>-1.1227979200000002E-6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="W1:AB1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>